<commit_message>
fix: permanent auth fix - use onAuthStateChange instead of getSession
Key changes:
- Remove getSession() with timeout approach (caused loading issues)
- Use onAuthStateChange INITIAL_SESSION event (instant, no network call)
- Add isInitialized flag to distinguish loading from no-session states
- Add profile caching to reduce database calls
- Add unique storageKey for session persistence
- Update all pages to use isInitialized instead of authLoading
</commit_message>
<xml_diff>
--- a/Resources/ifrs17_questions_choices_explanations_chosen.xlsx
+++ b/Resources/ifrs17_questions_choices_explanations_chosen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin Ochieng\OneDrive - Kenbright\Attachments\projects\2025\November\IFRS 17 Exam App\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kenbright-my.sharepoint.com/personal/rochieng_kenbright_africa/Documents/Attachments/projects/2025/November/IFRS 17 Exam App/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{46502E9A-3E4A-4EB1-9F74-916293D4848D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IFRS17 Questions" sheetId="1" state="hidden" r:id="rId1"/>
@@ -5173,8 +5173,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>